<commit_message>
Add quote to csv
</commit_message>
<xml_diff>
--- a/Network Diargram.xlsx
+++ b/Network Diargram.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aukin\P300\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5463CCC8-12D4-4059-B826-3DA642E83255}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E299AAA0-F681-4A65-BE4B-473D8A286A16}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="462" windowWidth="25602" windowHeight="15540" activeTab="1" xr2:uid="{7DFC015A-26E8-427C-8DA4-F09B8E758443}"/>
+    <workbookView xWindow="0" yWindow="462" windowWidth="25602" windowHeight="15540" xr2:uid="{7DFC015A-26E8-427C-8DA4-F09B8E758443}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -454,10 +454,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -774,7 +775,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68399EE6-4F4C-4EE9-96E3-9050B01220A3}">
   <dimension ref="A1:E76"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -784,20 +787,20 @@
     <col min="5" max="5" width="13.62890625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>126</v>
       </c>
     </row>
@@ -2079,6 +2082,7 @@
   </sheetData>
   <autoFilter ref="A1:E76" xr:uid="{028A0A20-7778-4AB0-8149-30FF41A91235}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2086,13 +2090,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B0A1DC0-3C40-A848-8B6A-2ED129D83A79}">
   <dimension ref="A1:C206"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.9453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.3125" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Add single quote to  csv
</commit_message>
<xml_diff>
--- a/Network Diargram.xlsx
+++ b/Network Diargram.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aukin\P300\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E299AAA0-F681-4A65-BE4B-473D8A286A16}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03A1F118-5834-4802-AAE3-3A21327BEB12}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="462" windowWidth="25602" windowHeight="15540" xr2:uid="{7DFC015A-26E8-427C-8DA4-F09B8E758443}"/>
   </bookViews>
@@ -776,7 +776,7 @@
   <dimension ref="A1:E76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>

<commit_message>
Fix cyp to get csv from Github raw url
</commit_message>
<xml_diff>
--- a/Network Diargram.xlsx
+++ b/Network Diargram.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aukin\P300\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B2C8B3B-2DE6-47BD-99C2-BF7D9D4D9055}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C469362-CFB3-47A8-9A59-53EC6F83EE3A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="462" windowWidth="25602" windowHeight="15540" activeTab="2" xr2:uid="{7DFC015A-26E8-427C-8DA4-F09B8E758443}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1976" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1976" uniqueCount="131">
   <si>
     <t>Country</t>
   </si>
@@ -422,6 +422,9 @@
   </si>
   <si>
     <t>SourceCompnayName</t>
+  </si>
+  <si>
+    <t>SourceCompanyName</t>
   </si>
 </sst>
 </file>
@@ -4979,17 +4982,18 @@
   <dimension ref="A1:E246"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
+    <col min="1" max="1" width="20.68359375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.15625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>128</v>

</xml_diff>